<commit_message>
Laatste ontbrekende comments toegevoegd
</commit_message>
<xml_diff>
--- a/clanoverview_logs/generated_reports/2017-12-27_clanlog.xlsx
+++ b/clanoverview_logs/generated_reports/2017-12-27_clanlog.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="105">
   <si>
     <t>Rank</t>
   </si>
@@ -68,6 +68,12 @@
     <t>leader</t>
   </si>
   <si>
+    <t>bastaard</t>
+  </si>
+  <si>
+    <t>#2JGULJY8</t>
+  </si>
+  <si>
     <t>clan de renzo</t>
   </si>
   <si>
@@ -80,12 +86,6 @@
     <t>#QR2VVJJG</t>
   </si>
   <si>
-    <t>bastaard</t>
-  </si>
-  <si>
-    <t>#2JGULJY8</t>
-  </si>
-  <si>
     <t>Bam</t>
   </si>
   <si>
@@ -104,16 +104,52 @@
     <t>#V8QY2UUJ</t>
   </si>
   <si>
+    <t>GJS</t>
+  </si>
+  <si>
+    <t>#8YJRVRLC</t>
+  </si>
+  <si>
     <t>shag tand</t>
   </si>
   <si>
     <t>#90VUQ988</t>
   </si>
   <si>
-    <t>GJS</t>
-  </si>
-  <si>
-    <t>#8YJRVRLC</t>
+    <t>tomtoch</t>
+  </si>
+  <si>
+    <t>#8299JUJY</t>
+  </si>
+  <si>
+    <t>wht^</t>
+  </si>
+  <si>
+    <t>#QU0VGY9</t>
+  </si>
+  <si>
+    <t>leeuw</t>
+  </si>
+  <si>
+    <t>#PP0C92QP</t>
+  </si>
+  <si>
+    <t>* haakie *</t>
+  </si>
+  <si>
+    <t>#2CUU0VJG</t>
+  </si>
+  <si>
+    <t>Z!P</t>
+  </si>
+  <si>
+    <t>#YVYU9Y8R</t>
+  </si>
+  <si>
+    <t>Ronald O</t>
+  </si>
+  <si>
+    <t>#99UJ999G</t>
   </si>
   <si>
     <t>xavier</t>
@@ -122,42 +158,6 @@
     <t>#8P88LUCQ</t>
   </si>
   <si>
-    <t>wht^</t>
-  </si>
-  <si>
-    <t>#QU0VGY9</t>
-  </si>
-  <si>
-    <t>tomtoch</t>
-  </si>
-  <si>
-    <t>#8299JUJY</t>
-  </si>
-  <si>
-    <t>leeuw</t>
-  </si>
-  <si>
-    <t>#PP0C92QP</t>
-  </si>
-  <si>
-    <t>* haakie *</t>
-  </si>
-  <si>
-    <t>#2CUU0VJG</t>
-  </si>
-  <si>
-    <t>Z!P</t>
-  </si>
-  <si>
-    <t>#YVYU9Y8R</t>
-  </si>
-  <si>
-    <t>Ronald O</t>
-  </si>
-  <si>
-    <t>#99UJ999G</t>
-  </si>
-  <si>
     <t>THICK GIRLS</t>
   </si>
   <si>
@@ -203,6 +203,12 @@
     <t>#22GU992L</t>
   </si>
   <si>
+    <t>BlackWing</t>
+  </si>
+  <si>
+    <t>#PJ8CG2J9</t>
+  </si>
+  <si>
     <t>peter</t>
   </si>
   <si>
@@ -221,12 +227,6 @@
     <t>#GYVQ0Y8R</t>
   </si>
   <si>
-    <t>BlackWing</t>
-  </si>
-  <si>
-    <t>#PJ8CG2J9</t>
-  </si>
-  <si>
     <t>mauzer99</t>
   </si>
   <si>
@@ -287,22 +287,34 @@
     <t>#9CGP2Y2G</t>
   </si>
   <si>
+    <t>SUPREMACYYYY</t>
+  </si>
+  <si>
+    <t>#8VP0J2QP</t>
+  </si>
+  <si>
+    <t>ergo</t>
+  </si>
+  <si>
+    <t>#QR2LJQY</t>
+  </si>
+  <si>
+    <t>OhhJayky!</t>
+  </si>
+  <si>
+    <t>#R0Y2J8G2</t>
+  </si>
+  <si>
     <t>jojo</t>
   </si>
   <si>
     <t>#22G9G88CC</t>
   </si>
   <si>
-    <t>OhhJayky!</t>
-  </si>
-  <si>
-    <t>#R0Y2J8G2</t>
-  </si>
-  <si>
-    <t>SUPREMACYYYY</t>
-  </si>
-  <si>
-    <t>#8VP0J2QP</t>
+    <t>Ergo460</t>
+  </si>
+  <si>
+    <t>#98LPPUJQ</t>
   </si>
   <si>
     <t>Duke en wes</t>
@@ -451,19 +463,19 @@
         <v>178.0</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>5086.0</v>
+        <v>5138.0</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>1532.0</v>
+        <v>1816.0</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>1202.0</v>
+        <v>1461.0</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>1.27</v>
+        <v>1.24</v>
       </c>
     </row>
     <row r="3">
@@ -480,19 +492,19 @@
         <v>198.0</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>5059.0</v>
+        <v>5070.0</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G3" s="3" t="n">
-        <v>1022.0</v>
+        <v>1112.0</v>
       </c>
       <c r="H3" s="3" t="n">
-        <v>369.0</v>
+        <v>441.0</v>
       </c>
       <c r="I3" s="3" t="n">
-        <v>2.77</v>
+        <v>2.52</v>
       </c>
     </row>
     <row r="4">
@@ -515,13 +527,13 @@
         <v>17</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>447.0</v>
+        <v>487.0</v>
       </c>
       <c r="H4" s="2" t="n">
         <v>370.0</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>1.21</v>
+        <v>1.32</v>
       </c>
     </row>
     <row r="5">
@@ -535,22 +547,22 @@
         <v>19</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>180.0</v>
+        <v>210.0</v>
       </c>
       <c r="E5" s="3" t="n">
-        <v>4983.0</v>
+        <v>4991.0</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G5" s="3" t="n">
-        <v>324.0</v>
+        <v>733.0</v>
       </c>
       <c r="H5" s="3" t="n">
-        <v>440.0</v>
+        <v>695.0</v>
       </c>
       <c r="I5" s="3" t="n">
-        <v>0.74</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="6">
@@ -564,22 +576,22 @@
         <v>21</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>189.0</v>
+        <v>180.0</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>4978.0</v>
+        <v>4985.0</v>
       </c>
       <c r="F6" t="s">
         <v>14</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>84.0</v>
+        <v>324.0</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>558.0</v>
+        <v>512.0</v>
       </c>
       <c r="I6" s="2" t="n">
-        <v>0.15</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="7">
@@ -593,22 +605,22 @@
         <v>23</v>
       </c>
       <c r="D7" s="3" t="n">
-        <v>210.0</v>
+        <v>189.0</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>4967.0</v>
+        <v>4978.0</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G7" s="3" t="n">
-        <v>651.0</v>
+        <v>84.0</v>
       </c>
       <c r="H7" s="3" t="n">
-        <v>584.0</v>
+        <v>558.0</v>
       </c>
       <c r="I7" s="3" t="n">
-        <v>1.11</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="8">
@@ -631,13 +643,13 @@
         <v>14</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>114.0</v>
+        <v>230.0</v>
       </c>
       <c r="H8" s="2" t="n">
         <v>97.0</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>1.18</v>
+        <v>2.37</v>
       </c>
     </row>
     <row r="9">
@@ -654,19 +666,19 @@
         <v>172.0</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>4911.0</v>
+        <v>4924.0</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G9" s="3" t="n">
-        <v>504.0</v>
+        <v>646.0</v>
       </c>
       <c r="H9" s="3" t="n">
-        <v>331.0</v>
+        <v>479.0</v>
       </c>
       <c r="I9" s="3" t="n">
-        <v>1.52</v>
+        <v>1.35</v>
       </c>
     </row>
     <row r="10">
@@ -683,7 +695,7 @@
         <v>179.0</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>4869.0</v>
+        <v>4859.0</v>
       </c>
       <c r="F10" t="s">
         <v>14</v>
@@ -692,10 +704,10 @@
         <v>576.0</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>329.0</v>
+        <v>364.0</v>
       </c>
       <c r="I10" s="2" t="n">
-        <v>1.75</v>
+        <v>1.58</v>
       </c>
     </row>
     <row r="11">
@@ -709,22 +721,22 @@
         <v>31</v>
       </c>
       <c r="D11" s="3" t="n">
-        <v>184.0</v>
+        <v>162.0</v>
       </c>
       <c r="E11" s="3" t="n">
-        <v>4847.0</v>
+        <v>4853.0</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G11" s="3" t="n">
-        <v>262.0</v>
+        <v>182.0</v>
       </c>
       <c r="H11" s="3" t="n">
-        <v>77.0</v>
+        <v>331.0</v>
       </c>
       <c r="I11" s="3" t="n">
-        <v>3.4</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="12">
@@ -738,22 +750,22 @@
         <v>33</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>162.0</v>
+        <v>184.0</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>4843.0</v>
+        <v>4847.0</v>
       </c>
       <c r="F12" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G12" s="2" t="n">
-        <v>177.0</v>
+        <v>277.0</v>
       </c>
       <c r="H12" s="2" t="n">
-        <v>294.0</v>
+        <v>77.0</v>
       </c>
       <c r="I12" s="2" t="n">
-        <v>0.6</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="13">
@@ -767,22 +779,22 @@
         <v>35</v>
       </c>
       <c r="D13" s="3" t="n">
-        <v>182.0</v>
+        <v>180.0</v>
       </c>
       <c r="E13" s="3" t="n">
-        <v>4837.0</v>
+        <v>4841.0</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G13" s="3" t="n">
-        <v>614.0</v>
+        <v>225.0</v>
       </c>
       <c r="H13" s="3" t="n">
-        <v>702.0</v>
+        <v>333.0</v>
       </c>
       <c r="I13" s="3" t="n">
-        <v>0.87</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="14">
@@ -799,19 +811,19 @@
         <v>175.0</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>4832.0</v>
+        <v>4831.0</v>
       </c>
       <c r="F14" t="s">
         <v>14</v>
       </c>
       <c r="G14" s="2" t="n">
-        <v>226.0</v>
+        <v>340.0</v>
       </c>
       <c r="H14" s="2" t="n">
-        <v>255.0</v>
+        <v>292.0</v>
       </c>
       <c r="I14" s="2" t="n">
-        <v>0.89</v>
+        <v>1.16</v>
       </c>
     </row>
     <row r="15">
@@ -825,22 +837,22 @@
         <v>39</v>
       </c>
       <c r="D15" s="3" t="n">
-        <v>180.0</v>
+        <v>175.0</v>
       </c>
       <c r="E15" s="3" t="n">
-        <v>4831.0</v>
+        <v>4790.0</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G15" s="3" t="n">
-        <v>215.0</v>
+        <v>469.0</v>
       </c>
       <c r="H15" s="3" t="n">
-        <v>296.0</v>
+        <v>498.0</v>
       </c>
       <c r="I15" s="3" t="n">
-        <v>0.73</v>
+        <v>0.94</v>
       </c>
     </row>
     <row r="16">
@@ -854,22 +866,22 @@
         <v>41</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>175.0</v>
+        <v>170.0</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>4790.0</v>
+        <v>4705.0</v>
       </c>
       <c r="F16" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G16" s="2" t="n">
-        <v>469.0</v>
+        <v>979.0</v>
       </c>
       <c r="H16" s="2" t="n">
-        <v>498.0</v>
+        <v>406.0</v>
       </c>
       <c r="I16" s="2" t="n">
-        <v>0.94</v>
+        <v>2.41</v>
       </c>
     </row>
     <row r="17">
@@ -883,22 +895,22 @@
         <v>43</v>
       </c>
       <c r="D17" s="3" t="n">
-        <v>170.0</v>
+        <v>179.0</v>
       </c>
       <c r="E17" s="3" t="n">
-        <v>4757.0</v>
+        <v>4702.0</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G17" s="3" t="n">
-        <v>747.0</v>
+        <v>157.0</v>
       </c>
       <c r="H17" s="3" t="n">
-        <v>297.0</v>
+        <v>140.0</v>
       </c>
       <c r="I17" s="3" t="n">
-        <v>2.52</v>
+        <v>1.12</v>
       </c>
     </row>
     <row r="18">
@@ -912,22 +924,22 @@
         <v>45</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>179.0</v>
+        <v>163.0</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>4733.0</v>
+        <v>4632.0</v>
       </c>
       <c r="F18" t="s">
         <v>14</v>
       </c>
       <c r="G18" s="2" t="n">
-        <v>155.0</v>
+        <v>368.0</v>
       </c>
       <c r="H18" s="2" t="n">
-        <v>105.0</v>
+        <v>646.0</v>
       </c>
       <c r="I18" s="2" t="n">
-        <v>1.48</v>
+        <v>0.57</v>
       </c>
     </row>
     <row r="19">
@@ -941,22 +953,22 @@
         <v>47</v>
       </c>
       <c r="D19" s="3" t="n">
-        <v>163.0</v>
+        <v>182.0</v>
       </c>
       <c r="E19" s="3" t="n">
-        <v>4631.0</v>
+        <v>4609.0</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G19" s="3" t="n">
-        <v>353.0</v>
+        <v>800.0</v>
       </c>
       <c r="H19" s="3" t="n">
-        <v>609.0</v>
+        <v>860.0</v>
       </c>
       <c r="I19" s="3" t="n">
-        <v>0.58</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="20">
@@ -973,7 +985,7 @@
         <v>184.0</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>4589.0</v>
+        <v>4584.0</v>
       </c>
       <c r="F20" t="s">
         <v>14</v>
@@ -1002,7 +1014,7 @@
         <v>192.0</v>
       </c>
       <c r="E21" s="3" t="n">
-        <v>4504.0</v>
+        <v>4532.0</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>11</v>
@@ -1031,19 +1043,19 @@
         <v>211.0</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>4494.0</v>
+        <v>4493.0</v>
       </c>
       <c r="F22" t="s">
         <v>14</v>
       </c>
       <c r="G22" s="2" t="n">
-        <v>394.0</v>
+        <v>416.0</v>
       </c>
       <c r="H22" s="2" t="n">
-        <v>1250.0</v>
+        <v>1329.0</v>
       </c>
       <c r="I22" s="2" t="n">
-        <v>0.32</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="23">
@@ -1089,7 +1101,7 @@
         <v>161.0</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>4443.0</v>
+        <v>4440.0</v>
       </c>
       <c r="F24" t="s">
         <v>56</v>
@@ -1147,19 +1159,19 @@
         <v>175.0</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>4410.0</v>
+        <v>4399.0</v>
       </c>
       <c r="F26" t="s">
         <v>14</v>
       </c>
       <c r="G26" s="2" t="n">
-        <v>431.0</v>
+        <v>492.0</v>
       </c>
       <c r="H26" s="2" t="n">
-        <v>636.0</v>
+        <v>706.0</v>
       </c>
       <c r="I26" s="2" t="n">
-        <v>0.68</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="27">
@@ -1176,19 +1188,19 @@
         <v>160.0</v>
       </c>
       <c r="E27" s="3" t="n">
-        <v>4295.0</v>
+        <v>4269.0</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G27" s="3" t="n">
-        <v>131.0</v>
+        <v>72.0</v>
       </c>
       <c r="H27" s="3" t="n">
-        <v>259.0</v>
+        <v>227.0</v>
       </c>
       <c r="I27" s="3" t="n">
-        <v>0.51</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="28">
@@ -1202,22 +1214,22 @@
         <v>66</v>
       </c>
       <c r="D28" s="2" t="n">
-        <v>195.0</v>
+        <v>160.0</v>
       </c>
       <c r="E28" s="2" t="n">
-        <v>4259.0</v>
+        <v>4262.0</v>
       </c>
       <c r="F28" t="s">
         <v>14</v>
       </c>
       <c r="G28" s="2" t="n">
-        <v>921.0</v>
+        <v>180.0</v>
       </c>
       <c r="H28" s="2" t="n">
-        <v>852.0</v>
+        <v>313.0</v>
       </c>
       <c r="I28" s="2" t="n">
-        <v>1.08</v>
+        <v>0.58</v>
       </c>
     </row>
     <row r="29">
@@ -1231,22 +1243,22 @@
         <v>68</v>
       </c>
       <c r="D29" s="3" t="n">
-        <v>178.0</v>
+        <v>195.0</v>
       </c>
       <c r="E29" s="3" t="n">
-        <v>4228.0</v>
+        <v>4259.0</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G29" s="3" t="n">
-        <v>66.0</v>
+        <v>951.0</v>
       </c>
       <c r="H29" s="3" t="n">
-        <v>148.0</v>
+        <v>852.0</v>
       </c>
       <c r="I29" s="3" t="n">
-        <v>0.45</v>
+        <v>1.12</v>
       </c>
     </row>
     <row r="30">
@@ -1260,22 +1272,22 @@
         <v>70</v>
       </c>
       <c r="D30" s="2" t="n">
-        <v>160.0</v>
+        <v>178.0</v>
       </c>
       <c r="E30" s="2" t="n">
-        <v>4216.0</v>
+        <v>4233.0</v>
       </c>
       <c r="F30" t="s">
         <v>14</v>
       </c>
       <c r="G30" s="2" t="n">
-        <v>35.0</v>
+        <v>126.0</v>
       </c>
       <c r="H30" s="2" t="n">
-        <v>153.0</v>
+        <v>222.0</v>
       </c>
       <c r="I30" s="2" t="n">
-        <v>0.23</v>
+        <v>0.57</v>
       </c>
     </row>
     <row r="31">
@@ -1321,19 +1333,19 @@
         <v>146.0</v>
       </c>
       <c r="E32" s="2" t="n">
-        <v>4120.0</v>
+        <v>4121.0</v>
       </c>
       <c r="F32" t="s">
         <v>56</v>
       </c>
       <c r="G32" s="2" t="n">
-        <v>137.0</v>
+        <v>288.0</v>
       </c>
       <c r="H32" s="2" t="n">
-        <v>183.0</v>
+        <v>329.0</v>
       </c>
       <c r="I32" s="2" t="n">
-        <v>0.75</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="33">
@@ -1350,19 +1362,19 @@
         <v>168.0</v>
       </c>
       <c r="E33" s="3" t="n">
-        <v>3819.0</v>
+        <v>3842.0</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G33" s="3" t="n">
-        <v>135.0</v>
+        <v>177.0</v>
       </c>
       <c r="H33" s="3" t="n">
-        <v>322.0</v>
+        <v>430.0</v>
       </c>
       <c r="I33" s="3" t="n">
-        <v>0.42</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="34">
@@ -1379,19 +1391,19 @@
         <v>156.0</v>
       </c>
       <c r="E34" s="2" t="n">
-        <v>3806.0</v>
+        <v>3803.0</v>
       </c>
       <c r="F34" t="s">
         <v>11</v>
       </c>
       <c r="G34" s="2" t="n">
-        <v>271.0</v>
+        <v>283.0</v>
       </c>
       <c r="H34" s="2" t="n">
         <v>140.0</v>
       </c>
       <c r="I34" s="2" t="n">
-        <v>1.94</v>
+        <v>2.02</v>
       </c>
     </row>
     <row r="35">
@@ -1408,19 +1420,19 @@
         <v>171.0</v>
       </c>
       <c r="E35" s="3" t="n">
-        <v>3717.0</v>
+        <v>3726.0</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G35" s="3" t="n">
-        <v>736.0</v>
+        <v>847.0</v>
       </c>
       <c r="H35" s="3" t="n">
-        <v>465.0</v>
+        <v>573.0</v>
       </c>
       <c r="I35" s="3" t="n">
-        <v>1.58</v>
+        <v>1.48</v>
       </c>
     </row>
     <row r="36">
@@ -1437,7 +1449,7 @@
         <v>159.0</v>
       </c>
       <c r="E36" s="2" t="n">
-        <v>3611.0</v>
+        <v>3598.0</v>
       </c>
       <c r="F36" t="s">
         <v>56</v>
@@ -1466,19 +1478,19 @@
         <v>166.0</v>
       </c>
       <c r="E37" s="3" t="n">
-        <v>3389.0</v>
+        <v>3435.0</v>
       </c>
       <c r="F37" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G37" s="3" t="n">
-        <v>329.0</v>
+        <v>504.0</v>
       </c>
       <c r="H37" s="3" t="n">
-        <v>287.0</v>
+        <v>413.0</v>
       </c>
       <c r="I37" s="3" t="n">
-        <v>1.15</v>
+        <v>1.22</v>
       </c>
     </row>
     <row r="38">
@@ -1559,13 +1571,13 @@
         <v>11</v>
       </c>
       <c r="G40" s="2" t="n">
-        <v>823.0</v>
+        <v>872.0</v>
       </c>
       <c r="H40" s="2" t="n">
         <v>915.0</v>
       </c>
       <c r="I40" s="2" t="n">
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="41">
@@ -1579,22 +1591,22 @@
         <v>92</v>
       </c>
       <c r="D41" s="3" t="n">
-        <v>156.0</v>
+        <v>152.0</v>
       </c>
       <c r="E41" s="3" t="n">
-        <v>3238.0</v>
+        <v>3248.0</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="G41" s="3" t="n">
-        <v>372.0</v>
+        <v>302.0</v>
       </c>
       <c r="H41" s="3" t="n">
-        <v>917.0</v>
+        <v>460.0</v>
       </c>
       <c r="I41" s="3" t="n">
-        <v>0.41</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="42">
@@ -1608,22 +1620,22 @@
         <v>94</v>
       </c>
       <c r="D42" s="2" t="n">
-        <v>123.0</v>
+        <v>154.0</v>
       </c>
       <c r="E42" s="2" t="n">
-        <v>3199.0</v>
+        <v>3211.0</v>
       </c>
       <c r="F42" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G42" s="2" t="n">
-        <v>69.0</v>
+        <v>4.0</v>
       </c>
       <c r="H42" s="2" t="n">
-        <v>62.0</v>
+        <v>35.0</v>
       </c>
       <c r="I42" s="2" t="n">
-        <v>1.11</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="43">
@@ -1637,22 +1649,22 @@
         <v>96</v>
       </c>
       <c r="D43" s="3" t="n">
-        <v>152.0</v>
+        <v>123.0</v>
       </c>
       <c r="E43" s="3" t="n">
-        <v>3159.0</v>
+        <v>3199.0</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="G43" s="3" t="n">
-        <v>272.0</v>
+        <v>69.0</v>
       </c>
       <c r="H43" s="3" t="n">
-        <v>354.0</v>
+        <v>62.0</v>
       </c>
       <c r="I43" s="3" t="n">
-        <v>0.77</v>
+        <v>1.11</v>
       </c>
     </row>
     <row r="44">
@@ -1666,22 +1678,22 @@
         <v>98</v>
       </c>
       <c r="D44" s="2" t="n">
-        <v>113.0</v>
+        <v>156.0</v>
       </c>
       <c r="E44" s="2" t="n">
-        <v>2577.0</v>
+        <v>3113.0</v>
       </c>
       <c r="F44" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G44" s="2" t="n">
-        <v>124.0</v>
+        <v>407.0</v>
       </c>
       <c r="H44" s="2" t="n">
-        <v>184.0</v>
+        <v>988.0</v>
       </c>
       <c r="I44" s="2" t="n">
-        <v>0.67</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="45">
@@ -1695,28 +1707,86 @@
         <v>100</v>
       </c>
       <c r="D45" s="3" t="n">
-        <v>69.0</v>
+        <v>136.0</v>
       </c>
       <c r="E45" s="3" t="n">
-        <v>1333.0</v>
+        <v>2656.0</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="G45" s="3" t="n">
         <v>0.0</v>
       </c>
       <c r="H45" s="3" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="I45" s="3" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="B46" t="s">
+        <v>101</v>
+      </c>
+      <c r="C46" t="s">
+        <v>102</v>
+      </c>
+      <c r="D46" s="2" t="n">
+        <v>113.0</v>
+      </c>
+      <c r="E46" s="2" t="n">
+        <v>2577.0</v>
+      </c>
+      <c r="F46" t="s">
+        <v>14</v>
+      </c>
+      <c r="G46" s="2" t="n">
+        <v>124.0</v>
+      </c>
+      <c r="H46" s="2" t="n">
+        <v>184.0</v>
+      </c>
+      <c r="I46" s="2" t="n">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="3" t="n">
+        <v>46.0</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D47" s="3" t="n">
+        <v>69.0</v>
+      </c>
+      <c r="E47" s="3" t="n">
+        <v>1333.0</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G47" s="3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H47" s="3" t="n">
         <v>40.0</v>
       </c>
-      <c r="I45" s="3" t="n">
+      <c r="I47" s="3" t="n">
         <v>0.0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.5" footer="0.3" header="0.3" left="0.25" right="0.25" top="0.5"/>
   <headerFooter>
-    <oddFooter>&amp;LClanoverzicht&amp;R27/12/2017 10:49</oddFooter>
+    <oddFooter>&amp;LClanoverzicht&amp;R27/12/2017 16:05</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>